<commit_message>
Amazon Star Rating logic
</commit_message>
<xml_diff>
--- a/data/Amazon_Product_data_all.xlsx
+++ b/data/Amazon_Product_data_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f943686c21a634a0/Desktop/Data Mining/CSCI-Final-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{B4CDE0A2-F8B9-4E6C-9F1C-8B4E1FA58B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AABFCDB-EDF3-44D5-955B-B3525A812FC1}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{B4CDE0A2-F8B9-4E6C-9F1C-8B4E1FA58B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E23D96A5-BBD9-4F53-A584-9D8619CA6605}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="131">
   <si>
     <t>productID</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>amazon12</t>
-  </si>
-  <si>
-    <t>https://a.co/d/c8Ghj92</t>
   </si>
   <si>
     <t>amazon13</t>
@@ -430,9 +427,6 @@
 Material Feature	Recycled</t>
   </si>
   <si>
-    <t>Doritos, Nacho Cheese Flavored Tortilla Chips Party Size, 15 oz</t>
-  </si>
-  <si>
     <t>Crest Cavity &amp; Tartar Protection Toothpaste, Whitening Baking Soda &amp; Peroxide, 5.7 oz, Pack of 2</t>
   </si>
   <si>
@@ -441,14 +435,6 @@
 Whitens teeth by removing surface stains
 Gentle on tooth enamel
 Freshens breath for a clean feeling mouth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Brand	Crest
-Flavor	Mint
-Age Range (Description)	Adult
-Item Form	Paste
-Target Audience	Unisex Adults</t>
   </si>
   <si>
     <t>OXO Good Grips 3-PC Small Square Short POP Container Set, White,Grey</t>
@@ -669,6 +655,29 @@
 Leg Length	4 Inches
 Type	Sofa Chaise
 Color	Blue/Gray</t>
+  </si>
+  <si>
+    <t>https://a.co/d/70GLQPp</t>
+  </si>
+  <si>
+    <t>Doritos Flavored Tortilla Chips, Spicy Sweet Chili, 42 Ounce (Pack of 4)</t>
+  </si>
+  <si>
+    <t>If your tongue is torn between choosing spicy or sweet, give it a delicious tango of Doritos spicy sweet chili flavored tortilla chips. Each bite is a mouth-watering, tooth-rattling crunch of delicious sweet and spicy flavor. Combine the Doritos crunch with a combination of spicy and sweet, and you’ve got an unstoppably delicious snack. Grab a bag and stock up on the bold taste of Doritos spicy sweet chili tortilla chips.</t>
+  </si>
+  <si>
+    <t>Brand	Crest
+Flavor	Mint
+Age Range (Description)	Adult
+Item Form	Paste
+Target Audience	Unisex Adults</t>
+  </si>
+  <si>
+    <t>Flavor Name: Sweet Chilli
+Size: 2.63 Pound (Pack of 4)Product Dimensions ‏ : ‎ 16.2 x 12.5 x 10.6 inches; 2.63 Pounds
+UPC ‏ : ‎ 028400337274
+Manufacturer ‏ : ‎ Frito Lay Products
+ASIN ‏ : ‎ B00T8AW9Z2</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1075,8 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="F2:G2"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1129,13 +1138,13 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="H2" s="1">
         <v>4.2</v>
@@ -1161,13 +1170,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="H3" s="1">
         <v>4.2</v>
@@ -1193,13 +1202,13 @@
         <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H4" s="1">
         <v>4.0999999999999996</v>
@@ -1225,13 +1234,13 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H5" s="1">
         <v>4.8</v>
@@ -1257,13 +1266,13 @@
         <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H6" s="1">
         <v>4.4000000000000004</v>
@@ -1289,13 +1298,13 @@
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="H7" s="1">
         <v>3.4</v>
@@ -1321,13 +1330,13 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="H8" s="1">
         <v>4.3</v>
@@ -1353,13 +1362,13 @@
         <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="H9" s="1">
         <v>4.5999999999999996</v>
@@ -1385,13 +1394,13 @@
         <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="H10" s="1">
         <v>4.5999999999999996</v>
@@ -1417,13 +1426,13 @@
         <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="H11" s="1">
         <v>4.2</v>
@@ -1449,13 +1458,13 @@
         <v>32</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="H12" s="1">
         <v>4.8</v>
@@ -1467,7 +1476,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1478,10 +1487,25 @@
         <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>91</v>
+        <v>127</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>187</v>
+      </c>
+      <c r="J13" s="1">
+        <v>28.99</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="87" x14ac:dyDescent="0.35">
@@ -1489,22 +1513,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="H14" s="1">
         <v>4.8</v>
@@ -1521,22 +1545,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H15" s="1">
         <v>4.5999999999999996</v>
@@ -1553,22 +1577,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="H16" s="1">
         <v>4.7</v>
@@ -1585,22 +1609,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="H17" s="1">
         <v>4.5999999999999996</v>
@@ -1617,22 +1641,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="H18" s="1">
         <v>4.9000000000000004</v>
@@ -1649,22 +1673,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="H19" s="1">
         <v>4.5999999999999996</v>
@@ -1681,22 +1705,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="H20" s="1">
         <v>4.4000000000000004</v>
@@ -1713,22 +1737,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H21" s="1">
         <v>4.4000000000000004</v>
@@ -1745,22 +1769,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H22" s="1">
         <v>4.4000000000000004</v>
@@ -1777,22 +1801,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H23" s="1">
         <v>4.2</v>
@@ -1809,22 +1833,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H24" s="1">
         <v>4.5</v>
@@ -1841,22 +1865,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H25" s="1">
         <v>4</v>

</xml_diff>